<commit_message>
Update vak vezet vilagtalant.xlsx
nekem ezek nem jók
</commit_message>
<xml_diff>
--- a/vak vezet vilagtalant.xlsx
+++ b/vak vezet vilagtalant.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VIZSGAREMEK\Vizsgaremek-D-K-B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Asztali gép\Minden is\Suli\github\Vizsgaremek-D-K-B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597F0E33-BCD2-475A-8B91-47F9E5481D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E6EA86CA-E58C-4D75-AC13-17473B008D05}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IP címek" sheetId="1" r:id="rId1"/>
@@ -527,7 +526,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1302,7 +1301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1580,27 +1579,63 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1619,34 +1654,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1697,16 +1708,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2027,7 +2035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B758846-9D45-4F65-A4A7-543A1E8CEAFB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2051,34 +2059,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="136" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="122" t="s">
+      <c r="B1" s="136"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="123"/>
+      <c r="E1" s="135"/>
       <c r="H1" s="41" t="s">
         <v>89</v>
       </c>
       <c r="I1" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="115" t="s">
+      <c r="J1" s="119" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="116"/>
+      <c r="K1" s="120"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="120"/>
+      <c r="C2" s="131"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="H2" s="28" t="s">
@@ -2098,8 +2106,8 @@
       <c r="A3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="118"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="133"/>
       <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2121,10 +2129,10 @@
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="120"/>
+      <c r="C4" s="131"/>
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="H4" s="29" t="s">
@@ -2155,10 +2163,10 @@
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="129"/>
+      <c r="C6" s="123"/>
       <c r="D6" s="22" t="s">
         <v>17</v>
       </c>
@@ -2168,32 +2176,32 @@
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="129"/>
+      <c r="C7" s="123"/>
       <c r="D7" s="22" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="130" t="s">
+      <c r="A8" s="140" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="127"/>
+      <c r="C8" s="139"/>
       <c r="D8" s="6"/>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="131"/>
-      <c r="B9" s="117" t="s">
+      <c r="A9" s="141"/>
+      <c r="B9" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="118"/>
+      <c r="C9" s="133"/>
       <c r="D9" s="7" t="s">
         <v>25</v>
       </c>
@@ -2220,7 +2228,7 @@
       <c r="A11" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="132" t="s">
+      <c r="B11" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -2232,21 +2240,21 @@
       <c r="E11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="115" t="s">
+      <c r="H11" s="119" t="s">
         <v>151</v>
       </c>
       <c r="I11" s="121"/>
-      <c r="J11" s="116"/>
-      <c r="K11" s="115" t="s">
+      <c r="J11" s="120"/>
+      <c r="K11" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="116"/>
+      <c r="L11" s="120"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="133"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="11" t="s">
         <v>38</v>
       </c>
@@ -2259,10 +2267,10 @@
       <c r="H12" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="128" t="s">
+      <c r="I12" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="129"/>
+      <c r="J12" s="123"/>
       <c r="K12" s="26" t="s">
         <v>8</v>
       </c>
@@ -2272,7 +2280,7 @@
       <c r="A13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="134"/>
+      <c r="B13" s="126"/>
       <c r="C13" s="13" t="s">
         <v>39</v>
       </c>
@@ -2285,10 +2293,10 @@
       <c r="H13" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="128" t="s">
+      <c r="I13" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="J13" s="129"/>
+      <c r="J13" s="123"/>
       <c r="K13" s="26" t="s">
         <v>8</v>
       </c>
@@ -2298,37 +2306,37 @@
       <c r="H14" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="I14" s="128" t="s">
+      <c r="I14" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="129"/>
+      <c r="J14" s="123"/>
       <c r="K14" s="26" t="s">
         <v>8</v>
       </c>
       <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H15" s="135" t="s">
+      <c r="H15" s="127" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="119" t="s">
+      <c r="I15" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="120"/>
+      <c r="J15" s="131"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="115" t="s">
+      <c r="A16" s="119" t="s">
         <v>104</v>
       </c>
       <c r="B16" s="121"/>
-      <c r="C16" s="116"/>
+      <c r="C16" s="120"/>
       <c r="D16" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="116"/>
-      <c r="H16" s="136"/>
+      <c r="E16" s="120"/>
+      <c r="H16" s="128"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8" t="s">
         <v>8</v>
@@ -2342,13 +2350,13 @@
       <c r="A17" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="119" t="s">
+      <c r="B17" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="120"/>
+      <c r="C17" s="131"/>
       <c r="D17" s="3"/>
       <c r="E17" s="14"/>
-      <c r="H17" s="136"/>
+      <c r="H17" s="128"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10" t="s">
         <v>63</v>
@@ -2362,13 +2370,13 @@
       <c r="A18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="118"/>
+      <c r="B18" s="132"/>
+      <c r="C18" s="133"/>
       <c r="D18" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="H18" s="136"/>
+      <c r="H18" s="128"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10" t="s">
         <v>64</v>
@@ -2382,13 +2390,13 @@
       <c r="A19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="119" t="s">
+      <c r="B19" s="130" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="120"/>
+      <c r="C19" s="131"/>
       <c r="D19" s="3"/>
       <c r="E19" s="14"/>
-      <c r="H19" s="136"/>
+      <c r="H19" s="128"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10" t="s">
         <v>65</v>
@@ -2402,13 +2410,13 @@
       <c r="A20" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="118"/>
+      <c r="B20" s="132"/>
+      <c r="C20" s="133"/>
       <c r="D20" s="22" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="H20" s="137"/>
+      <c r="H20" s="129"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12" t="s">
         <v>66</v>
@@ -2422,16 +2430,16 @@
       <c r="A21" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="120"/>
+      <c r="C21" s="131"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="H21" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="132" t="s">
+      <c r="I21" s="124" t="s">
         <v>26</v>
       </c>
       <c r="J21" s="31" t="s">
@@ -2446,10 +2454,10 @@
       <c r="A22" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="118"/>
+      <c r="C22" s="133"/>
       <c r="D22" s="5" t="s">
         <v>33</v>
       </c>
@@ -2457,7 +2465,7 @@
       <c r="H22" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="I22" s="133"/>
+      <c r="I22" s="125"/>
       <c r="J22" s="21" t="s">
         <v>2</v>
       </c>
@@ -2485,7 +2493,7 @@
       <c r="H23" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="I23" s="134"/>
+      <c r="I23" s="126"/>
       <c r="J23" s="32" t="s">
         <v>68</v>
       </c>
@@ -2498,7 +2506,7 @@
       <c r="A24" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="132" t="s">
+      <c r="B24" s="124" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -2513,7 +2521,7 @@
       <c r="H24" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="I24" s="132" t="s">
+      <c r="I24" s="124" t="s">
         <v>13</v>
       </c>
       <c r="J24" s="31" t="s">
@@ -2530,7 +2538,7 @@
       <c r="A25" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="133"/>
+      <c r="B25" s="125"/>
       <c r="C25" s="10" t="s">
         <v>41</v>
       </c>
@@ -2543,7 +2551,7 @@
       <c r="H25" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="I25" s="133"/>
+      <c r="I25" s="125"/>
       <c r="J25" s="21" t="s">
         <v>81</v>
       </c>
@@ -2558,7 +2566,7 @@
       <c r="A26" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="134"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="12" t="s">
         <v>42</v>
       </c>
@@ -2571,7 +2579,7 @@
       <c r="H26" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="I26" s="134"/>
+      <c r="I26" s="126"/>
       <c r="J26" s="32" t="s">
         <v>82</v>
       </c>
@@ -2619,20 +2627,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="H15:H20"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B24:B26"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B17:C17"/>
@@ -2649,6 +2643,20 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B11:B13"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="H15:H20"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2657,7 +2665,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C9080C5-0883-4588-929C-C2F43E02CFA4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2678,11 +2686,11 @@
       <c r="A2" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="145" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="143"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="147"/>
       <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2736,11 +2744,11 @@
       <c r="A7" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="142" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
+      <c r="C7" s="143"/>
+      <c r="D7" s="143"/>
       <c r="F7" s="64"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2811,11 +2819,11 @@
       <c r="A14" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="138" t="s">
+      <c r="B14" s="142" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="139"/>
-      <c r="D14" s="140"/>
+      <c r="C14" s="143"/>
+      <c r="D14" s="144"/>
       <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2918,11 +2926,11 @@
       <c r="A23" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="138" t="s">
+      <c r="B23" s="142" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="139"/>
-      <c r="D23" s="140"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="144"/>
       <c r="F23" s="64"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2997,11 +3005,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADE9CDE-7E54-481D-8CA0-47D915E8AF28}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,28 +3022,28 @@
   <sheetData>
     <row r="1" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L2" s="150" t="s">
+      <c r="L2" s="154" t="s">
         <v>159</v>
       </c>
-      <c r="M2" s="151"/>
-      <c r="N2" s="152"/>
-      <c r="O2" s="152"/>
-      <c r="P2" s="152"/>
-      <c r="Q2" s="152"/>
-      <c r="R2" s="152"/>
-      <c r="S2" s="152"/>
-      <c r="T2" s="153"/>
+      <c r="M2" s="155"/>
+      <c r="N2" s="156"/>
+      <c r="O2" s="156"/>
+      <c r="P2" s="156"/>
+      <c r="Q2" s="156"/>
+      <c r="R2" s="156"/>
+      <c r="S2" s="156"/>
+      <c r="T2" s="157"/>
     </row>
     <row r="3" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="144" t="s">
+      <c r="C3" s="148" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="145"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="145"/>
-      <c r="G3" s="145"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="146"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="150"/>
       <c r="L3" s="109" t="s">
         <v>160</v>
       </c>
@@ -3131,28 +3139,28 @@
       <c r="F7" s="83">
         <v>27</v>
       </c>
-      <c r="G7" s="90">
+      <c r="G7" s="158">
         <v>28</v>
       </c>
-      <c r="H7" s="94">
+      <c r="H7" s="159">
         <v>1</v>
       </c>
-      <c r="I7" s="84">
+      <c r="I7" s="160">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="3:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="147" t="s">
+      <c r="C10" s="151" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="148"/>
-      <c r="E10" s="148"/>
-      <c r="F10" s="148"/>
-      <c r="G10" s="148"/>
-      <c r="H10" s="148"/>
-      <c r="I10" s="149"/>
+      <c r="D10" s="152"/>
+      <c r="E10" s="152"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="152"/>
+      <c r="H10" s="152"/>
+      <c r="I10" s="153"/>
     </row>
     <row r="11" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="104" t="s">
@@ -3191,25 +3199,25 @@
       </c>
     </row>
     <row r="13" spans="3:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="154">
+      <c r="C13" s="115">
         <v>3</v>
       </c>
-      <c r="D13" s="155">
+      <c r="D13" s="116">
         <v>4</v>
       </c>
-      <c r="E13" s="155">
+      <c r="E13" s="116">
         <v>5</v>
       </c>
-      <c r="F13" s="155">
+      <c r="F13" s="116">
         <v>6</v>
       </c>
-      <c r="G13" s="156">
+      <c r="G13" s="117">
         <v>7</v>
       </c>
-      <c r="H13" s="154">
+      <c r="H13" s="115">
         <v>8</v>
       </c>
-      <c r="I13" s="157">
+      <c r="I13" s="118">
         <v>9</v>
       </c>
       <c r="K13" t="s">
@@ -3311,15 +3319,15 @@
     <row r="18" spans="3:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="3:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="147" t="s">
+      <c r="C20" s="151" t="s">
         <v>140</v>
       </c>
-      <c r="D20" s="148"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="148"/>
-      <c r="H20" s="148"/>
-      <c r="I20" s="149"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="152"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="153"/>
     </row>
     <row r="21" spans="3:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="104" t="s">

</xml_diff>

<commit_message>
ospf elvileg jó, majd nézzétek át
</commit_message>
<xml_diff>
--- a/vak vezet vilagtalant.xlsx
+++ b/vak vezet vilagtalant.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VIZSGAREMEK\Vizsgaremek-D-K-B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Asztali gép\Minden is\Suli\github\Vizsgaremek-D-K-B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B257A5-3966-4947-929B-5FFA6871E188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13230" yWindow="525" windowWidth="21480" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13230" yWindow="525" windowWidth="21480" windowHeight="11400" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IP címek" sheetId="1" r:id="rId1"/>
@@ -785,7 +784,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1913,85 +1912,85 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2348,10 +2347,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
@@ -2375,35 +2374,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="141" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="145" t="s">
+      <c r="B1" s="141"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="146"/>
+      <c r="E1" s="140"/>
       <c r="H1" s="24" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="133" t="s">
+      <c r="J1" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="135"/>
+      <c r="K1" s="128"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="125" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="122" t="s">
+      <c r="C2" s="134"/>
+      <c r="D2" s="143" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3"/>
@@ -2421,10 +2420,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="137"/>
-      <c r="B3" s="126"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="123"/>
+      <c r="A3" s="126"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="144"/>
       <c r="E3" s="5"/>
       <c r="H3" s="17" t="s">
         <v>22</v>
@@ -2440,14 +2439,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="129" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="122" t="s">
+      <c r="C4" s="134"/>
+      <c r="D4" s="143" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="4"/>
@@ -2465,10 +2464,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="137"/>
-      <c r="B5" s="126"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="123"/>
+      <c r="A5" s="126"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="135"/>
+      <c r="D5" s="144"/>
       <c r="E5" s="4"/>
       <c r="H5" s="16" t="s">
         <v>181</v>
@@ -2485,10 +2484,10 @@
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="132"/>
+      <c r="C6" s="147"/>
       <c r="D6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2505,14 +2504,14 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="136" t="s">
+      <c r="A7" s="125" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="124" t="s">
+      <c r="B7" s="129" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="122" t="s">
+      <c r="C7" s="134"/>
+      <c r="D7" s="143" t="s">
         <v>128</v>
       </c>
       <c r="E7" s="95" t="s">
@@ -2530,10 +2529,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="137"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="127"/>
-      <c r="D8" s="123"/>
+      <c r="A8" s="126"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="135"/>
+      <c r="D8" s="144"/>
       <c r="E8" s="96"/>
       <c r="H8" s="115" t="s">
         <v>189</v>
@@ -2547,30 +2546,30 @@
       <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="136" t="s">
+      <c r="A9" s="125" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="124" t="s">
+      <c r="B9" s="129" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="125"/>
-      <c r="D9" s="138" t="s">
+      <c r="C9" s="134"/>
+      <c r="D9" s="124" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="137"/>
-      <c r="B10" s="126"/>
-      <c r="C10" s="128"/>
-      <c r="D10" s="138"/>
+      <c r="A10" s="126"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="145"/>
+      <c r="D10" s="124"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="124" t="s">
+      <c r="B11" s="129" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="100" t="s">
@@ -2587,7 +2586,7 @@
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="139"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="8" t="s">
         <v>134</v>
       </c>
@@ -2602,7 +2601,7 @@
       <c r="A13" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="126"/>
+      <c r="B13" s="131"/>
       <c r="C13" s="99" t="s">
         <v>193</v>
       </c>
@@ -2615,24 +2614,24 @@
     </row>
     <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="133" t="s">
+      <c r="A15" s="127" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="134"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="133" t="s">
+      <c r="B15" s="148"/>
+      <c r="C15" s="128"/>
+      <c r="D15" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="135"/>
+      <c r="E15" s="128"/>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B16" s="129" t="s">
+      <c r="B16" s="122" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="130"/>
+      <c r="C16" s="123"/>
       <c r="D16" s="15" t="s">
         <v>154</v>
       </c>
@@ -2642,10 +2641,10 @@
       <c r="A17" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="129" t="s">
+      <c r="B17" s="122" t="s">
         <v>166</v>
       </c>
-      <c r="C17" s="130"/>
+      <c r="C17" s="123"/>
       <c r="D17" s="15" t="s">
         <v>5</v>
       </c>
@@ -2655,10 +2654,10 @@
       <c r="A18" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="B18" s="129" t="s">
+      <c r="B18" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="130"/>
+      <c r="C18" s="123"/>
       <c r="D18" s="15" t="s">
         <v>154</v>
       </c>
@@ -2668,7 +2667,7 @@
       <c r="A19" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="B19" s="124" t="s">
+      <c r="B19" s="129" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="100" t="s">
@@ -2685,7 +2684,7 @@
       <c r="A20" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B20" s="139"/>
+      <c r="B20" s="130"/>
       <c r="C20" s="8" t="s">
         <v>172</v>
       </c>
@@ -2700,7 +2699,7 @@
       <c r="A21" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="B21" s="126"/>
+      <c r="B21" s="131"/>
       <c r="C21" s="99" t="s">
         <v>176</v>
       </c>
@@ -2713,24 +2712,24 @@
     </row>
     <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="144" t="s">
+      <c r="A23" s="138" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="142"/>
-      <c r="C23" s="143"/>
-      <c r="D23" s="142" t="s">
+      <c r="B23" s="136"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="143"/>
+      <c r="E23" s="137"/>
     </row>
     <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="129" t="s">
+      <c r="B24" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="130"/>
+      <c r="C24" s="123"/>
       <c r="D24" s="110" t="s">
         <v>154</v>
       </c>
@@ -2742,10 +2741,10 @@
       <c r="A25" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="140" t="s">
+      <c r="B25" s="132" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="141"/>
+      <c r="C25" s="133"/>
       <c r="D25" s="96" t="s">
         <v>154</v>
       </c>
@@ -2753,7 +2752,7 @@
     </row>
     <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="97"/>
-      <c r="B26" s="124" t="s">
+      <c r="B26" s="129" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="100"/>
@@ -2762,21 +2761,21 @@
     </row>
     <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="139"/>
+      <c r="B27" s="130"/>
       <c r="C27" s="8"/>
       <c r="D27" s="11"/>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="139"/>
+      <c r="B28" s="130"/>
       <c r="C28" s="8"/>
       <c r="D28" s="11"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="98"/>
-      <c r="B29" s="126"/>
+      <c r="B29" s="131"/>
       <c r="C29" s="99"/>
       <c r="D29" s="12"/>
       <c r="E29" s="7"/>
@@ -3302,6 +3301,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D15:E15"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="A4:A5"/>
@@ -3318,18 +3329,6 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3338,11 +3337,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3431,7 +3430,7 @@
       <c r="C5" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="105" t="s">
         <v>41</v>
       </c>
       <c r="E5" s="74"/>
@@ -3446,7 +3445,7 @@
       <c r="C6" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="105" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="74"/>
@@ -3710,11 +3709,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
vtp, hsrp, ether channel,
raah
</commit_message>
<xml_diff>
--- a/vak vezet vilagtalant.xlsx
+++ b/vak vezet vilagtalant.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Asztali gép\Minden is\Suli\github\Vizsgaremek-D-K-B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VIZSGAREMEK\Vizsgaremek-D-K-B\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2705A870-6604-4CCE-A386-A6AE185156F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13230" yWindow="525" windowWidth="21480" windowHeight="11400" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IP címek" sheetId="1" r:id="rId1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="258">
   <si>
     <t>192.168.1.0</t>
   </si>
@@ -779,12 +780,42 @@
   </si>
   <si>
     <t>192.168.2.158</t>
+  </si>
+  <si>
+    <t>192.168.2.161</t>
+  </si>
+  <si>
+    <t>192.168.2.162</t>
+  </si>
+  <si>
+    <t>192.168.2.163</t>
+  </si>
+  <si>
+    <t>voice</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>wireless</t>
+  </si>
+  <si>
+    <t>192.168.3.24</t>
+  </si>
+  <si>
+    <t>192.168.3.28</t>
+  </si>
+  <si>
+    <t>192.168.3.23</t>
+  </si>
+  <si>
+    <t>192.168.3.27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1912,48 +1943,66 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1973,24 +2022,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2347,11 +2378,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2374,35 +2405,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="147" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="139" t="s">
+      <c r="B1" s="147"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="140"/>
+      <c r="E1" s="146"/>
       <c r="H1" s="24" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="127" t="s">
+      <c r="J1" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="128"/>
+      <c r="K1" s="135"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="136" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="143" t="s">
+      <c r="C2" s="125"/>
+      <c r="D2" s="122" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3"/>
@@ -2420,10 +2451,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="126"/>
-      <c r="B3" s="131"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="144"/>
+      <c r="A3" s="137"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="123"/>
       <c r="E3" s="5"/>
       <c r="H3" s="17" t="s">
         <v>22</v>
@@ -2439,14 +2470,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="129" t="s">
+      <c r="B4" s="124" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="134"/>
-      <c r="D4" s="143" t="s">
+      <c r="C4" s="125"/>
+      <c r="D4" s="122" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="4"/>
@@ -2464,10 +2495,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="126"/>
-      <c r="B5" s="131"/>
-      <c r="C5" s="135"/>
-      <c r="D5" s="144"/>
+      <c r="A5" s="137"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="123"/>
       <c r="E5" s="4"/>
       <c r="H5" s="16" t="s">
         <v>181</v>
@@ -2484,10 +2515,10 @@
       <c r="A6" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="146" t="s">
+      <c r="B6" s="131" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="147"/>
+      <c r="C6" s="132"/>
       <c r="D6" s="13" t="s">
         <v>4</v>
       </c>
@@ -2504,14 +2535,14 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="136" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="124" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="134"/>
-      <c r="D7" s="143" t="s">
+      <c r="C7" s="125"/>
+      <c r="D7" s="122" t="s">
         <v>128</v>
       </c>
       <c r="E7" s="95" t="s">
@@ -2529,10 +2560,10 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="126"/>
-      <c r="B8" s="131"/>
-      <c r="C8" s="135"/>
-      <c r="D8" s="144"/>
+      <c r="A8" s="137"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="127"/>
+      <c r="D8" s="123"/>
       <c r="E8" s="96"/>
       <c r="H8" s="115" t="s">
         <v>189</v>
@@ -2546,30 +2577,30 @@
       <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="125" t="s">
+      <c r="A9" s="136" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="129" t="s">
+      <c r="B9" s="124" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="134"/>
-      <c r="D9" s="124" t="s">
+      <c r="C9" s="125"/>
+      <c r="D9" s="138" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="126"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="145"/>
-      <c r="D10" s="124"/>
+      <c r="A10" s="137"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="138"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="129" t="s">
+      <c r="B11" s="124" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="100" t="s">
@@ -2586,7 +2617,7 @@
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="130"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="8" t="s">
         <v>134</v>
       </c>
@@ -2601,7 +2632,7 @@
       <c r="A13" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="131"/>
+      <c r="B13" s="126"/>
       <c r="C13" s="99" t="s">
         <v>193</v>
       </c>
@@ -2614,24 +2645,24 @@
     </row>
     <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="127" t="s">
+      <c r="A15" s="133" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="148"/>
-      <c r="C15" s="128"/>
-      <c r="D15" s="127" t="s">
+      <c r="B15" s="134"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="128"/>
+      <c r="E15" s="135"/>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="B16" s="122" t="s">
+      <c r="B16" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="123"/>
+      <c r="C16" s="130"/>
       <c r="D16" s="15" t="s">
         <v>154</v>
       </c>
@@ -2641,10 +2672,10 @@
       <c r="A17" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="B17" s="122" t="s">
+      <c r="B17" s="129" t="s">
         <v>166</v>
       </c>
-      <c r="C17" s="123"/>
+      <c r="C17" s="130"/>
       <c r="D17" s="15" t="s">
         <v>5</v>
       </c>
@@ -2654,10 +2685,10 @@
       <c r="A18" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="B18" s="122" t="s">
+      <c r="B18" s="129" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="123"/>
+      <c r="C18" s="130"/>
       <c r="D18" s="15" t="s">
         <v>154</v>
       </c>
@@ -2667,7 +2698,7 @@
       <c r="A19" s="97" t="s">
         <v>171</v>
       </c>
-      <c r="B19" s="129" t="s">
+      <c r="B19" s="124" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="100" t="s">
@@ -2684,7 +2715,7 @@
       <c r="A20" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B20" s="130"/>
+      <c r="B20" s="139"/>
       <c r="C20" s="8" t="s">
         <v>172</v>
       </c>
@@ -2699,7 +2730,7 @@
       <c r="A21" s="98" t="s">
         <v>179</v>
       </c>
-      <c r="B21" s="131"/>
+      <c r="B21" s="126"/>
       <c r="C21" s="99" t="s">
         <v>176</v>
       </c>
@@ -2712,24 +2743,24 @@
     </row>
     <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="138" t="s">
+      <c r="A23" s="144" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="136"/>
-      <c r="C23" s="137"/>
-      <c r="D23" s="136" t="s">
+      <c r="B23" s="142"/>
+      <c r="C23" s="143"/>
+      <c r="D23" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="137"/>
+      <c r="E23" s="143"/>
     </row>
     <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="122" t="s">
+      <c r="B24" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="123"/>
+      <c r="C24" s="130"/>
       <c r="D24" s="110" t="s">
         <v>154</v>
       </c>
@@ -2741,10 +2772,10 @@
       <c r="A25" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="132" t="s">
+      <c r="B25" s="140" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="133"/>
+      <c r="C25" s="141"/>
       <c r="D25" s="96" t="s">
         <v>154</v>
       </c>
@@ -2752,7 +2783,7 @@
     </row>
     <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="97"/>
-      <c r="B26" s="129" t="s">
+      <c r="B26" s="124" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="100"/>
@@ -2761,21 +2792,21 @@
     </row>
     <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="130"/>
+      <c r="B27" s="139"/>
       <c r="C27" s="8"/>
       <c r="D27" s="11"/>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="130"/>
+      <c r="B28" s="139"/>
       <c r="C28" s="8"/>
       <c r="D28" s="11"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="98"/>
-      <c r="B29" s="131"/>
+      <c r="B29" s="126"/>
       <c r="C29" s="99"/>
       <c r="D29" s="12"/>
       <c r="E29" s="7"/>
@@ -3298,21 +3329,121 @@
       <c r="C57" s="22" t="s">
         <v>233</v>
       </c>
+      <c r="D57" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>249</v>
+      </c>
+      <c r="F57" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="H57" s="22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="B60" s="22">
+        <v>16</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" s="22">
+        <v>1</v>
+      </c>
+      <c r="E60" s="22">
+        <v>14</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="G60" s="22">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B61" s="22">
+        <v>8</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="22">
+        <v>17</v>
+      </c>
+      <c r="E61" s="22">
+        <v>22</v>
+      </c>
+      <c r="F61" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="G61" s="22">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B62" s="22">
+        <v>4</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D62" s="22">
+        <v>25</v>
+      </c>
+      <c r="E62" s="22">
+        <v>26</v>
+      </c>
+      <c r="F62" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="G62" s="22">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B63" s="22">
+        <v>4</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="D63" s="22">
+        <v>29</v>
+      </c>
+      <c r="E63" s="22">
+        <v>30</v>
+      </c>
+      <c r="F63" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="G63" s="22">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="22" t="s">
+        <v>142</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="A4:A5"/>
@@ -3329,6 +3460,18 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3337,11 +3480,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3442,7 +3585,7 @@
       <c r="B6" s="121" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="92" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="105" t="s">
@@ -3457,7 +3600,7 @@
       <c r="B7" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="80" t="s">
+      <c r="C7" s="92" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="81" t="s">
@@ -3472,7 +3615,7 @@
       <c r="B8" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="92" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="81" t="s">
@@ -3487,7 +3630,7 @@
       <c r="B9" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="92" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="81" t="s">
@@ -3709,7 +3852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">

</xml_diff>

<commit_message>
nat + tunnel teszt
</commit_message>
<xml_diff>
--- a/vak vezet vilagtalant.xlsx
+++ b/vak vezet vilagtalant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meste\OneDrive\Desktop\Új mappa\Vizsgaremek-D-K-B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180CB572-3942-47C7-BC39-7EDD0A4CE864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F85D14F-E6D8-49A7-994C-4C9ACFB511D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4530" yWindow="1305" windowWidth="14895" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,9 +311,6 @@
     <t>GRE + ipv6</t>
   </si>
   <si>
-    <t>vpn, home office</t>
-  </si>
-  <si>
     <t>wlc</t>
   </si>
   <si>
@@ -809,7 +806,10 @@
     <t>192.168.3.27</t>
   </si>
   <si>
-    <t>asa</t>
+    <t>asa, vpn, home office</t>
+  </si>
+  <si>
+    <t>portsecurity</t>
   </si>
 </sst>
 </file>
@@ -975,7 +975,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1592,24 +1592,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1836,9 +1823,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1980,48 +1964,66 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2041,24 +2043,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2442,35 +2426,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="149" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="149"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="147" t="s">
+      <c r="A1" s="154" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="154"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="148"/>
+      <c r="E1" s="153"/>
       <c r="H1" s="24" t="s">
         <v>15</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="135" t="s">
+      <c r="J1" s="140" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="136"/>
+      <c r="K1" s="142"/>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="133" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="137" t="s">
+      <c r="A2" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="142"/>
-      <c r="D2" s="151" t="s">
+      <c r="C2" s="132"/>
+      <c r="D2" s="129" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="3"/>
@@ -2488,10 +2472,10 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="134"/>
-      <c r="B3" s="139"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="152"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="130"/>
       <c r="E3" s="5"/>
       <c r="H3" s="17" t="s">
         <v>22</v>
@@ -2507,14 +2491,14 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="133" t="s">
+      <c r="A4" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="137" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="142"/>
-      <c r="D4" s="151" t="s">
+      <c r="B4" s="131" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="132"/>
+      <c r="D4" s="129" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="4"/>
@@ -2532,187 +2516,187 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="134"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="143"/>
-      <c r="D5" s="152"/>
+      <c r="A5" s="144"/>
+      <c r="B5" s="133"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="130"/>
       <c r="E5" s="4"/>
       <c r="H5" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="100"/>
+      <c r="J5" s="111" t="s">
         <v>180</v>
       </c>
-      <c r="I5" s="101"/>
-      <c r="J5" s="112" t="s">
-        <v>181</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="154" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="155"/>
+      <c r="C6" s="139"/>
       <c r="D6" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="15"/>
       <c r="H6" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6" s="101"/>
+      <c r="J6" s="112" t="s">
         <v>182</v>
       </c>
-      <c r="I6" s="102"/>
-      <c r="J6" s="113" t="s">
+      <c r="K6" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="K6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="143" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="131" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="132"/>
+      <c r="D7" s="129" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="94" t="s">
+        <v>190</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="133" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="137" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="142"/>
-      <c r="D7" s="151" t="s">
+      <c r="I7" s="102"/>
+      <c r="J7" s="113" t="s">
+        <v>185</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="144"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="134"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="95"/>
+      <c r="H8" s="114" t="s">
+        <v>187</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="115" t="s">
+        <v>189</v>
+      </c>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="143" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="95" t="s">
-        <v>191</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="I7" s="103"/>
-      <c r="J7" s="114" t="s">
-        <v>186</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="134"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="143"/>
-      <c r="D8" s="152"/>
-      <c r="E8" s="96"/>
-      <c r="H8" s="115" t="s">
-        <v>188</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="J8" s="116" t="s">
-        <v>190</v>
-      </c>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="133" t="s">
+      <c r="B9" s="131" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="137" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="142"/>
-      <c r="D9" s="132" t="s">
+      <c r="C9" s="132"/>
+      <c r="D9" s="145" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="134"/>
-      <c r="B10" s="139"/>
-      <c r="C10" s="153"/>
-      <c r="D10" s="132"/>
+      <c r="A10" s="144"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="135"/>
+      <c r="D10" s="145"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="137" t="s">
+      <c r="B11" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="100" t="s">
-        <v>132</v>
+      <c r="C11" s="99" t="s">
+        <v>131</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="138"/>
+      <c r="B12" s="146"/>
       <c r="C12" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="98" t="s">
+      <c r="A13" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="139"/>
-      <c r="C13" s="99" t="s">
-        <v>192</v>
+      <c r="B13" s="133"/>
+      <c r="C13" s="98" t="s">
+        <v>191</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="135" t="s">
-        <v>156</v>
-      </c>
-      <c r="B15" s="156"/>
-      <c r="C15" s="136"/>
-      <c r="D15" s="135" t="s">
+      <c r="A15" s="140" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="141"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="140" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="136"/>
+      <c r="E15" s="142"/>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="136" t="s">
         <v>162</v>
       </c>
-      <c r="B16" s="130" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16" s="131"/>
+      <c r="C16" s="137"/>
       <c r="D16" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="136" t="s">
         <v>164</v>
       </c>
-      <c r="B17" s="130" t="s">
-        <v>165</v>
-      </c>
-      <c r="C17" s="131"/>
+      <c r="C17" s="137"/>
       <c r="D17" s="15" t="s">
         <v>5</v>
       </c>
@@ -2720,131 +2704,131 @@
     </row>
     <row r="18" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="136" t="s">
         <v>166</v>
       </c>
-      <c r="B18" s="130" t="s">
+      <c r="C18" s="137"/>
+      <c r="D18" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="96" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="131" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="99" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="131"/>
-      <c r="D18" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="97" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="137" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="100" t="s">
+      <c r="D19" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>169</v>
-      </c>
       <c r="E19" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="138"/>
+        <v>178</v>
+      </c>
+      <c r="B20" s="146"/>
       <c r="C20" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="21" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="98" t="s">
-        <v>178</v>
-      </c>
-      <c r="B21" s="139"/>
-      <c r="C21" s="99" t="s">
+      <c r="A21" s="97" t="s">
+        <v>177</v>
+      </c>
+      <c r="B21" s="133"/>
+      <c r="C21" s="98" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="146" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="145"/>
-      <c r="D23" s="144" t="s">
+      <c r="A23" s="151" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="149"/>
+      <c r="C23" s="150"/>
+      <c r="D23" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="145"/>
+      <c r="E23" s="150"/>
     </row>
     <row r="24" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="109" t="s">
+      <c r="A24" s="108" t="s">
+        <v>151</v>
+      </c>
+      <c r="B24" s="136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="137"/>
+      <c r="D24" s="109" t="s">
         <v>152</v>
       </c>
-      <c r="B24" s="130" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="131"/>
-      <c r="D24" s="110" t="s">
+      <c r="E24" s="110" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="106" t="s">
         <v>153</v>
       </c>
-      <c r="E24" s="111" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="107" t="s">
-        <v>154</v>
-      </c>
-      <c r="B25" s="140" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="141"/>
-      <c r="D25" s="96" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="108"/>
+      <c r="B25" s="147" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="148"/>
+      <c r="D25" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="107"/>
     </row>
     <row r="26" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="97"/>
-      <c r="B26" s="137" t="s">
+      <c r="A26" s="96"/>
+      <c r="B26" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="100"/>
+      <c r="C26" s="99"/>
       <c r="D26" s="10"/>
       <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="138"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="8"/>
       <c r="D27" s="11"/>
       <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="138"/>
+      <c r="B28" s="146"/>
       <c r="C28" s="8"/>
       <c r="D28" s="11"/>
       <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:14" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="98"/>
-      <c r="B29" s="139"/>
-      <c r="C29" s="99"/>
+      <c r="A29" s="97"/>
+      <c r="B29" s="133"/>
+      <c r="C29" s="98"/>
       <c r="D29" s="12"/>
       <c r="E29" s="7"/>
     </row>
@@ -2854,14 +2838,14 @@
     </row>
     <row r="31" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K31" s="23"/>
       <c r="N31" s="23"/>
     </row>
     <row r="32" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" s="22">
         <v>32</v>
@@ -2870,100 +2854,100 @@
         <v>0</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K32" s="23"/>
       <c r="N32" s="23"/>
     </row>
     <row r="33" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B33" s="22">
         <v>32</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K33" s="23"/>
       <c r="N33" s="23"/>
     </row>
     <row r="34" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="22">
         <v>32</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D34" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="22" t="s">
-        <v>113</v>
-      </c>
       <c r="F34" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K34" s="23"/>
       <c r="N34" s="23"/>
     </row>
     <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" s="22">
         <v>16</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D35" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="E35" s="22" t="s">
-        <v>115</v>
-      </c>
       <c r="F35" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I35" s="23"/>
       <c r="L35" s="23"/>
@@ -2971,28 +2955,28 @@
     </row>
     <row r="36" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36" s="22">
         <v>16</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="22" t="s">
-        <v>117</v>
-      </c>
       <c r="F36" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I36" s="23"/>
       <c r="L36" s="23"/>
@@ -3000,28 +2984,28 @@
     </row>
     <row r="37" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B37" s="22">
         <v>16</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="22" t="s">
-        <v>119</v>
-      </c>
       <c r="F37" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I37" s="23"/>
       <c r="L37" s="23"/>
@@ -3029,90 +3013,90 @@
     </row>
     <row r="38" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="22">
         <v>16</v>
       </c>
       <c r="C38" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="D38" s="22" t="s">
         <v>203</v>
       </c>
-      <c r="D38" s="22" t="s">
-        <v>204</v>
-      </c>
       <c r="E38" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B39" s="22">
         <v>8</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D39" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="E39" s="22" t="s">
-        <v>221</v>
-      </c>
       <c r="F39" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B40" s="22">
         <v>4</v>
       </c>
       <c r="C40" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D40" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="E40" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="E40" s="22" t="s">
-        <v>219</v>
-      </c>
       <c r="F40" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G40" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H40" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="106" t="s">
-        <v>139</v>
+      <c r="A43" s="105" t="s">
+        <v>138</v>
       </c>
       <c r="B43" s="22">
         <v>16</v>
@@ -3121,94 +3105,94 @@
         <v>3</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G43" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H43" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B44" s="22">
         <v>16</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B45" s="22">
         <v>16</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D45" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E45" s="22" t="s">
-        <v>149</v>
-      </c>
       <c r="F45" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G45" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H45" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B51" s="22">
         <v>32</v>
@@ -3217,174 +3201,174 @@
         <v>2</v>
       </c>
       <c r="D51" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G51" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B52" s="22">
         <v>32</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D52" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G52" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B53" s="22">
         <v>32</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D53" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B54" s="22">
         <v>32</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D54" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E54" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B55" s="22">
         <v>16</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D55" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E55" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G55" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H55" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B56" s="22">
         <v>16</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E56" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H56" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C57" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D57" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="E57" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="E57" s="22" t="s">
+      <c r="F57" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="F57" s="22" t="s">
-        <v>249</v>
-      </c>
       <c r="G57" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H57" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B60" s="22">
         <v>16</v>
@@ -3399,7 +3383,7 @@
         <v>14</v>
       </c>
       <c r="F60" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G60" s="22">
         <v>240</v>
@@ -3407,13 +3391,13 @@
     </row>
     <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B61" s="22">
         <v>8</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D61" s="22">
         <v>17</v>
@@ -3422,7 +3406,7 @@
         <v>22</v>
       </c>
       <c r="F61" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G61" s="22">
         <v>248</v>
@@ -3430,13 +3414,13 @@
     </row>
     <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B62" s="22">
         <v>4</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D62" s="22">
         <v>25</v>
@@ -3445,7 +3429,7 @@
         <v>26</v>
       </c>
       <c r="F62" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G62" s="22">
         <v>252</v>
@@ -3453,13 +3437,13 @@
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B63" s="22">
         <v>4</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D63" s="22">
         <v>29</v>
@@ -3468,7 +3452,7 @@
         <v>30</v>
       </c>
       <c r="F63" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G63" s="22">
         <v>252</v>
@@ -3476,23 +3460,11 @@
     </row>
     <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C64" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B9:C10"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="A4:A5"/>
@@ -3509,6 +3481,18 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="B9:C10"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D15:E15"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3521,7 +3505,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3552,30 +3536,30 @@
       <c r="E1" s="74"/>
     </row>
     <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="157" t="s">
+      <c r="A2" s="156" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="117" t="s">
+      <c r="C2" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="103" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="74"/>
       <c r="F2" s="70"/>
-      <c r="G2" s="87" t="s">
+      <c r="G2" s="86" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="158"/>
-      <c r="B3" s="94" t="s">
+      <c r="A3" s="157"/>
+      <c r="B3" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="91" t="s">
         <v>80</v>
       </c>
       <c r="D3" s="81" t="s">
@@ -3583,61 +3567,61 @@
       </c>
       <c r="E3" s="74"/>
       <c r="F3" s="71"/>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="87" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="158"/>
+      <c r="A4" s="157"/>
       <c r="B4" s="79"/>
       <c r="C4" s="80"/>
-      <c r="D4" s="105" t="s">
+      <c r="D4" s="104" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="74"/>
       <c r="F4" s="72"/>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="88" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="120" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="104" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="74"/>
+    </row>
+    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="118" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="105" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="74"/>
-    </row>
-    <row r="6" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="85" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="121" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="104" t="s">
         <v>44</v>
       </c>
       <c r="E6" s="74"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="94" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="92" t="s">
+      <c r="B7" s="120" t="s">
+        <v>257</v>
+      </c>
+      <c r="C7" s="91" t="s">
         <v>37</v>
       </c>
       <c r="D7" s="81" t="s">
@@ -3646,13 +3630,13 @@
       <c r="E7" s="74"/>
     </row>
     <row r="8" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="85" t="s">
+      <c r="A8" s="84" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="94" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="92" t="s">
+      <c r="B8" s="120" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="91" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="81" t="s">
@@ -3661,13 +3645,13 @@
       <c r="E8" s="74"/>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="121" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="92" t="s">
+      <c r="B9" s="93" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="91" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="81" t="s">
@@ -3676,13 +3660,13 @@
       <c r="E9" s="74"/>
     </row>
     <row r="10" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="121" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="118" t="s">
+      <c r="B10" s="93" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="117" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="81" t="s">
@@ -3691,14 +3675,14 @@
       <c r="E10" s="74"/>
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="79" t="s">
-        <v>257</v>
+      <c r="B11" s="120" t="s">
+        <v>90</v>
       </c>
       <c r="C11" s="80" t="s">
-        <v>91</v>
+        <v>256</v>
       </c>
       <c r="D11" s="81" t="s">
         <v>85</v>
@@ -3706,14 +3690,14 @@
       <c r="E11" s="74"/>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="84" t="s">
         <v>70</v>
       </c>
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="120" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="81" t="s">
         <v>86</v>
@@ -3721,7 +3705,7 @@
       <c r="E12" s="74"/>
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="84" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="80"/>
@@ -3729,22 +3713,22 @@
       <c r="D13" s="81"/>
       <c r="E13" s="74"/>
     </row>
-    <row r="14" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="85" t="s">
+    <row r="14" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="82"/>
+      <c r="B14" s="80"/>
       <c r="C14" s="80"/>
       <c r="D14" s="81"/>
       <c r="E14" s="74"/>
     </row>
     <row r="15" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="86" t="s">
+      <c r="A15" s="85" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="82"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="84"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="83"/>
       <c r="E15" s="74"/>
     </row>
     <row r="16" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3906,26 +3890,26 @@
   <sheetData>
     <row r="2" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="159" t="s">
+      <c r="C3" s="158" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="161"/>
-      <c r="L3" s="165" t="s">
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="160"/>
+      <c r="L3" s="164" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="166"/>
-      <c r="N3" s="167"/>
-      <c r="O3" s="167"/>
-      <c r="P3" s="167"/>
-      <c r="Q3" s="167"/>
-      <c r="R3" s="167"/>
-      <c r="S3" s="167"/>
-      <c r="T3" s="168"/>
+      <c r="M3" s="165"/>
+      <c r="N3" s="166"/>
+      <c r="O3" s="166"/>
+      <c r="P3" s="166"/>
+      <c r="Q3" s="166"/>
+      <c r="R3" s="166"/>
+      <c r="S3" s="166"/>
+      <c r="T3" s="167"/>
     </row>
     <row r="4" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="44" t="s">
@@ -4015,7 +3999,7 @@
       <c r="D7" s="29">
         <v>25</v>
       </c>
-      <c r="E7" s="90">
+      <c r="E7" s="89">
         <v>26</v>
       </c>
       <c r="F7" s="29">
@@ -4027,22 +4011,22 @@
       <c r="H7" s="65">
         <v>1</v>
       </c>
-      <c r="I7" s="91">
+      <c r="I7" s="90">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="3:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="162" t="s">
+      <c r="C10" s="161" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="163"/>
-      <c r="E10" s="163"/>
-      <c r="F10" s="163"/>
-      <c r="G10" s="163"/>
-      <c r="H10" s="163"/>
-      <c r="I10" s="164"/>
+      <c r="D10" s="162"/>
+      <c r="E10" s="162"/>
+      <c r="F10" s="162"/>
+      <c r="G10" s="162"/>
+      <c r="H10" s="162"/>
+      <c r="I10" s="163"/>
     </row>
     <row r="11" spans="3:20" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="49" t="s">
@@ -4142,7 +4126,7 @@
       <c r="F15" s="25">
         <v>20</v>
       </c>
-      <c r="G15" s="120">
+      <c r="G15" s="119">
         <v>21</v>
       </c>
       <c r="H15" s="38">
@@ -4165,13 +4149,13 @@
       <c r="F16" s="25">
         <v>27</v>
       </c>
-      <c r="G16" s="122">
+      <c r="G16" s="121">
         <v>28</v>
       </c>
-      <c r="H16" s="123">
+      <c r="H16" s="122">
         <v>29</v>
       </c>
-      <c r="I16" s="124">
+      <c r="I16" s="123">
         <v>30</v>
       </c>
     </row>
@@ -4188,28 +4172,28 @@
       <c r="F17" s="29">
         <v>3</v>
       </c>
-      <c r="G17" s="125">
+      <c r="G17" s="124">
         <v>4</v>
       </c>
-      <c r="H17" s="126">
+      <c r="H17" s="125">
         <v>5</v>
       </c>
-      <c r="I17" s="127">
+      <c r="I17" s="126">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="3:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="162" t="s">
+      <c r="C20" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="163"/>
-      <c r="E20" s="163"/>
-      <c r="F20" s="163"/>
-      <c r="G20" s="163"/>
-      <c r="H20" s="163"/>
-      <c r="I20" s="164"/>
+      <c r="D20" s="162"/>
+      <c r="E20" s="162"/>
+      <c r="F20" s="162"/>
+      <c r="G20" s="162"/>
+      <c r="H20" s="162"/>
+      <c r="I20" s="163"/>
     </row>
     <row r="21" spans="3:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="49" t="s">
@@ -4259,7 +4243,7 @@
       <c r="C23" s="26">
         <v>7</v>
       </c>
-      <c r="D23" s="119">
+      <c r="D23" s="118">
         <v>8</v>
       </c>
       <c r="E23" s="25">
@@ -4291,10 +4275,10 @@
       <c r="F24" s="25">
         <v>17</v>
       </c>
-      <c r="G24" s="128">
+      <c r="G24" s="127">
         <v>18</v>
       </c>
-      <c r="H24" s="129">
+      <c r="H24" s="128">
         <v>19</v>
       </c>
       <c r="I24" s="27">

</xml_diff>